<commit_message>
- Rearanged all P#.. - Removed Keepout areas.. - Renamed all NM to DNP.. - Moved D1 from layer 16 to layer 1.. - Changed R8 from 0R NM to 0R.. - Placed more Grounding vias around RF connector in brd.. - Added two pullups res on I2C lines.. - Added the recomended filters on Tevo's power pins.. - Updated Document.. - Updated BOM..
</commit_message>
<xml_diff>
--- a/H1FR50/Released/BOM/H1FR50.xlsx
+++ b/H1FR50/Released/BOM/H1FR50.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Hexabitz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Hexabitz\H1FR5x-Hardware\H1FR50\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="152">
   <si>
     <t>Qty</t>
   </si>
@@ -276,27 +276,12 @@
     <t>C1, C6, C7, C8, C9</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>X7R SMD Chip Capacitor</t>
-  </si>
-  <si>
-    <t>GRM155R71C104KA88D</t>
-  </si>
-  <si>
-    <t>https://octopart.com/grm155r71c104ka88d-murata-196880?r=sp</t>
-  </si>
-  <si>
     <t>Taiyo Yuden</t>
   </si>
   <si>
     <t>C3, C4</t>
   </si>
   <si>
-    <t>C5</t>
-  </si>
-  <si>
     <t>1nF</t>
   </si>
   <si>
@@ -333,21 +318,6 @@
     <t>https://octopart.com/grm1555c1h560ja01d-murata-15197568?r=sp</t>
   </si>
   <si>
-    <t>100pF</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>GRM1555C1H101JA01D</t>
-  </si>
-  <si>
-    <t>0402 100pF 50V ±5 % Tolerance C0G SMT Multilayer Ceramic Capacitor</t>
-  </si>
-  <si>
-    <t>https://octopart.com/grm1555c1h101ja01d-murata-15197512?r=sp</t>
-  </si>
-  <si>
     <t>120pF</t>
   </si>
   <si>
@@ -358,9 +328,6 @@
   </si>
   <si>
     <t>https://octopart.com/grm1555c1h121ja01d-murata-196010?r=sp</t>
-  </si>
-  <si>
-    <t>C12</t>
   </si>
   <si>
     <t>C14</t>
@@ -467,27 +434,15 @@
     <t>https://octopart.com/crgcq0402f10k-te+connectivity-91017932?r=sp</t>
   </si>
   <si>
-    <t>3.0R</t>
-  </si>
-  <si>
     <t>AC0402FR-073RL</t>
   </si>
   <si>
     <t>https://octopart.com/ac0402fr-073rl-yageo-71366773?r=sp</t>
   </si>
   <si>
-    <t>0.0R NM</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
-    <t>R4, R10, R12</t>
-  </si>
-  <si>
-    <t>R6, R7, R8, R9, R11, R13</t>
-  </si>
-  <si>
     <t>R14</t>
   </si>
   <si>
@@ -561,6 +516,48 @@
   </si>
   <si>
     <t>1uF</t>
+  </si>
+  <si>
+    <t>C5, C11</t>
+  </si>
+  <si>
+    <t>C10, C12, C19</t>
+  </si>
+  <si>
+    <t>FB4</t>
+  </si>
+  <si>
+    <t>LQG15HS27NJ02D</t>
+  </si>
+  <si>
+    <t>Inductor RF Chip Multi-Layer 27nH 5% 100MHz 8Q-Factor Air 300mA 460mOhm DCR 0402 Paper T/R</t>
+  </si>
+  <si>
+    <t>https://octopart.com/lqg15hs27nj02d-murata-387555?r=sp</t>
+  </si>
+  <si>
+    <t>R6, R7, R9, R11, R13</t>
+  </si>
+  <si>
+    <t>R4, R8, R10, R12</t>
+  </si>
+  <si>
+    <t>0.0R DNP</t>
+  </si>
+  <si>
+    <t>3.0R DNP</t>
+  </si>
+  <si>
+    <t>2.2K</t>
+  </si>
+  <si>
+    <t>R15, R16</t>
+  </si>
+  <si>
+    <t>AC0402FR-072K2L</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ac0402fr-072k2l-yageo-24682183?r=sp</t>
   </si>
 </sst>
 </file>
@@ -638,7 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -651,9 +648,6 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -966,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,78 +1052,76 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>137</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4">
         <v>0.1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.1</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="2" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="2" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1137,23 +1129,23 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1161,23 +1153,25 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.1</v>
+      </c>
       <c r="H8" s="2" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1185,73 +1179,71 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0.1</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="G9" s="4"/>
       <c r="H9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1259,47 +1251,47 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="2" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1307,23 +1299,23 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1331,23 +1323,23 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1355,23 +1347,23 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="2" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1379,23 +1371,23 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="2" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1403,101 +1395,103 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>111</v>
+        <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="H18" s="2" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>10</v>
+        <v>145</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1505,51 +1499,51 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>121</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>148</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>29</v>
+        <v>150</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>30</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1584,22 +1578,22 @@
         <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1610,20 +1604,20 @@
         <v>734120110</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="F26" s="1">
         <v>734120110</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1655,23 +1649,23 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="2" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1679,23 +1673,23 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="2" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1703,23 +1697,23 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="2" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1727,23 +1721,23 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1773,15 +1767,14 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1"/>
-    <hyperlink ref="H5" r:id="rId2"/>
-    <hyperlink ref="H7" r:id="rId3"/>
-    <hyperlink ref="H14" r:id="rId4"/>
-    <hyperlink ref="H19" r:id="rId5"/>
-    <hyperlink ref="H4" r:id="rId6"/>
+    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="H6" r:id="rId3"/>
+    <hyperlink ref="H12" r:id="rId4"/>
+    <hyperlink ref="H18" r:id="rId5"/>
+    <hyperlink ref="H19" r:id="rId6"/>
     <hyperlink ref="H20" r:id="rId7"/>
-    <hyperlink ref="H21" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Redesigned both Schematic and PCB.. - Updated BOM and Documentation..
</commit_message>
<xml_diff>
--- a/H1FR50/Released/BOM/H1FR50.xlsx
+++ b/H1FR50/Released/BOM/H1FR50.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Hexabitz\H1FR5x-Hardware\H1FR50\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Current work\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="151">
   <si>
     <t>Qty</t>
   </si>
@@ -100,9 +100,6 @@
     <t>0.0R</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>Thick Film Resistors - SMD 0603</t>
   </si>
   <si>
@@ -127,12 +124,6 @@
     <t>R2</t>
   </si>
   <si>
-    <t>RC0603JR-0710KL</t>
-  </si>
-  <si>
-    <t>https://octopart.com/search?q=RC0603JR-0710KL&amp;start=0</t>
-  </si>
-  <si>
     <t>CAP CER  10% X7R 0603</t>
   </si>
   <si>
@@ -173,24 +164,6 @@
   </si>
   <si>
     <t>https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ</t>
-  </si>
-  <si>
-    <t>FB-TDK_MMZ1608Y300B</t>
-  </si>
-  <si>
-    <t>FB1</t>
-  </si>
-  <si>
-    <t>Ferrite Beads Multi-Layer 30Ohm 25% 100MHz 1.5A 50mOhm DCR 0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TDK </t>
-  </si>
-  <si>
-    <t>MMZ1608Y300B</t>
-  </si>
-  <si>
-    <t>https://octopart.com/mmz1608y300b-tdk-368280?r=sp&amp;s=cd9_2ZEqQ9q9UNBuQgHAiA</t>
   </si>
   <si>
     <t>PAD1</t>
@@ -273,15 +246,6 @@
     <t>Cap Tant Solid  SMD 2012</t>
   </si>
   <si>
-    <t>C1, C6, C7, C8, C9</t>
-  </si>
-  <si>
-    <t>Taiyo Yuden</t>
-  </si>
-  <si>
-    <t>C3, C4</t>
-  </si>
-  <si>
     <t>1nF</t>
   </si>
   <si>
@@ -339,22 +303,10 @@
     <t>C16</t>
   </si>
   <si>
-    <t>C2, C17</t>
-  </si>
-  <si>
     <t>2.2uF</t>
   </si>
   <si>
     <t>C18</t>
-  </si>
-  <si>
-    <t>EMK212B7225KGHT</t>
-  </si>
-  <si>
-    <t>https://octopart.com/emk212b7225kght-taiyo+yuden-29102998?r=sp</t>
-  </si>
-  <si>
-    <t>0805 2.2 uF 16 V ±10% Tolerance X7R Multilayer Ceramic Chip Capacitor</t>
   </si>
   <si>
     <t>ESDARF02-1BU2CK</t>
@@ -434,12 +386,6 @@
     <t>https://octopart.com/crgcq0402f10k-te+connectivity-91017932?r=sp</t>
   </si>
   <si>
-    <t>AC0402FR-073RL</t>
-  </si>
-  <si>
-    <t>https://octopart.com/ac0402fr-073rl-yageo-71366773?r=sp</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
@@ -515,15 +461,6 @@
     <t>https://octopart.com/teseo-liv3f-stmicroelectronics-84762432?r=sp</t>
   </si>
   <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>C5, C11</t>
-  </si>
-  <si>
-    <t>C10, C12, C19</t>
-  </si>
-  <si>
     <t>FB4</t>
   </si>
   <si>
@@ -545,19 +482,79 @@
     <t>0.0R DNP</t>
   </si>
   <si>
-    <t>3.0R DNP</t>
-  </si>
-  <si>
-    <t>2.2K</t>
-  </si>
-  <si>
-    <t>R15, R16</t>
-  </si>
-  <si>
-    <t>AC0402FR-072K2L</t>
-  </si>
-  <si>
-    <t>https://octopart.com/ac0402fr-072k2l-yageo-24682183?r=sp</t>
+    <t>C3, C5, C6, C8, C9</t>
+  </si>
+  <si>
+    <t>C4, C7</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>CGA2B3X7R1H103K050BE</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cga2b3x7r1h103k050be-tdk-68305469?r=sp</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 0.01uF 50V X7R 10% Pad SMD 0402 Soft Termination 125C Automotive T/R</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>AC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ac0603fr-07100kl-yageo-21711090?r=sp</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>1.00uF</t>
+  </si>
+  <si>
+    <t>C0402C105K8PAC7411</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 1uF 10V X5R 10% SMD 0402 85°C Paper T/R</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c0402c105k8pac7411-kemet-75146233?r=sp</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 2.2uF 4V X5R 10% SMD 0402 85°C Paper T/R</t>
+  </si>
+  <si>
+    <t>C0402C225K7PACTU</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c0402c225k7pactu-kemet-89187402?r=sp</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C10, C19</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 56pF 25V C0G 2% SMD 0201 125C Paper T/R</t>
+  </si>
+  <si>
+    <t>GRM0335C1E560GA01D</t>
+  </si>
+  <si>
+    <t>https://octopart.com/grm0335c1e560ga01d-murata-24611383?r=sp</t>
   </si>
 </sst>
 </file>
@@ -960,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,10 +979,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -997,7 +994,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -1011,13 +1008,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1029,51 +1026,51 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G3" s="4">
         <v>0.1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="4">
         <v>0.1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1081,47 +1078,47 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="2" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>61</v>
+        <v>143</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="2" t="s">
-        <v>34</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1129,23 +1126,23 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1153,25 +1150,23 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.1</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="2" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1179,71 +1174,73 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>131</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>130</v>
+      </c>
+      <c r="G9" s="1"/>
       <c r="H9" s="2" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>139</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.1</v>
+      </c>
       <c r="H10" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="2" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1251,71 +1248,71 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="G12" s="4"/>
       <c r="H12" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>149</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="2" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="G14" s="4"/>
       <c r="H14" s="2" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1323,23 +1320,23 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="2" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1347,23 +1344,23 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="2" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1371,23 +1368,23 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="2" t="s">
-        <v>143</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1395,103 +1392,99 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="G18" s="1"/>
       <c r="H18" s="2" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>105</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="G19" s="1"/>
       <c r="H19" s="2" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>146</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1499,51 +1492,51 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>148</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>103</v>
+        <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>150</v>
+        <v>26</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>105</v>
+        <v>49</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>151</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1551,23 +1544,23 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1575,25 +1568,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1604,20 +1597,20 @@
         <v>734120110</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F26" s="1">
         <v>734120110</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="2" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1631,7 +1624,7 @@
         <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>7</v>
@@ -1649,23 +1642,23 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="2" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1673,23 +1666,23 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="2" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1697,23 +1690,23 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="2" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1721,23 +1714,23 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1745,36 +1738,35 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1"/>
     <hyperlink ref="H4" r:id="rId2"/>
-    <hyperlink ref="H6" r:id="rId3"/>
-    <hyperlink ref="H12" r:id="rId4"/>
-    <hyperlink ref="H18" r:id="rId5"/>
-    <hyperlink ref="H19" r:id="rId6"/>
-    <hyperlink ref="H20" r:id="rId7"/>
+    <hyperlink ref="H7" r:id="rId3"/>
+    <hyperlink ref="H15" r:id="rId4"/>
+    <hyperlink ref="H20" r:id="rId5"/>
+    <hyperlink ref="H21" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Changed RF Connector.. - Documents and BOM were updated..
</commit_message>
<xml_diff>
--- a/H1FR50/Released/BOM/H1FR50.xlsx
+++ b/H1FR50/Released/BOM/H1FR50.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="152">
   <si>
     <t>Qty</t>
   </si>
@@ -437,12 +437,6 @@
     <t>Molex</t>
   </si>
   <si>
-    <t>https://octopart.com/0734120110-molex-16756629?r=sp&amp;s=MrVch9BMTneaw8n1KM-Tpw</t>
-  </si>
-  <si>
-    <t>Conn; RF/Coaxial; SMT; 50 Ohms; 1.25mm; Straight; Jack; Gold Plated</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -555,6 +549,15 @@
   </si>
   <si>
     <t>https://octopart.com/grm0335c1e560ga01d-murata-24611383?r=sp</t>
+  </si>
+  <si>
+    <t>732511150</t>
+  </si>
+  <si>
+    <t>https://octopart.com/73251-1150-molex-777272?r=sp</t>
+  </si>
+  <si>
+    <t>50 Ohms, SMA Jack Receptacle, Edge Mount, .25µm Gold (Au) Plating, One Piece Per Bag</t>
   </si>
 </sst>
 </file>
@@ -957,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1032,7 @@
         <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>18</v>
@@ -1052,10 +1055,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>52</v>
@@ -1078,23 +1081,23 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1108,17 +1111,17 @@
         <v>73</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1129,7 +1132,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>52</v>
@@ -1153,7 +1156,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>18</v>
@@ -1177,20 +1180,20 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1251,7 +1254,7 @@
         <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>63</v>
@@ -1275,20 +1278,20 @@
         <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1416,23 +1419,23 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1443,7 +1446,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>87</v>
@@ -1466,10 +1469,10 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>87</v>
@@ -1492,7 +1495,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>95</v>
@@ -1504,13 +1507,13 @@
         <v>11</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>89</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1593,24 +1596,24 @@
       <c r="A26" s="1">
         <v>1</v>
       </c>
-      <c r="B26" s="1">
-        <v>734120110</v>
+      <c r="B26" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F26" s="1">
-        <v>734120110</v>
+      <c r="F26" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="2" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1706,7 +1709,7 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1714,23 +1717,23 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- reconnected side pads to power..
</commit_message>
<xml_diff>
--- a/H1FR50/Released/BOM/H1FR50.xlsx
+++ b/H1FR50/Released/BOM/H1FR50.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Current work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Hexabitz\H1FR5x-Hardware\H1FR50\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -100,6 +100,9 @@
     <t>0.0R</t>
   </si>
   <si>
+    <t>R3</t>
+  </si>
+  <si>
     <t>Thick Film Resistors - SMD 0603</t>
   </si>
   <si>
@@ -124,6 +127,12 @@
     <t>R2</t>
   </si>
   <si>
+    <t>RC0603JR-0710KL</t>
+  </si>
+  <si>
+    <t>https://octopart.com/search?q=RC0603JR-0710KL&amp;start=0</t>
+  </si>
+  <si>
     <t>CAP CER  10% X7R 0603</t>
   </si>
   <si>
@@ -164,6 +173,24 @@
   </si>
   <si>
     <t>https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ</t>
+  </si>
+  <si>
+    <t>FB-TDK_MMZ1608Y300B</t>
+  </si>
+  <si>
+    <t>FB1</t>
+  </si>
+  <si>
+    <t>Ferrite Beads Multi-Layer 30Ohm 25% 100MHz 1.5A 50mOhm DCR 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDK </t>
+  </si>
+  <si>
+    <t>MMZ1608Y300B</t>
+  </si>
+  <si>
+    <t>https://octopart.com/mmz1608y300b-tdk-368280?r=sp&amp;s=cd9_2ZEqQ9q9UNBuQgHAiA</t>
   </si>
   <si>
     <t>PAD1</t>
@@ -246,6 +273,15 @@
     <t>Cap Tant Solid  SMD 2012</t>
   </si>
   <si>
+    <t>C1, C6, C7, C8, C9</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>C3, C4</t>
+  </si>
+  <si>
     <t>1nF</t>
   </si>
   <si>
@@ -303,10 +339,22 @@
     <t>C16</t>
   </si>
   <si>
+    <t>C2, C17</t>
+  </si>
+  <si>
     <t>2.2uF</t>
   </si>
   <si>
     <t>C18</t>
+  </si>
+  <si>
+    <t>EMK212B7225KGHT</t>
+  </si>
+  <si>
+    <t>https://octopart.com/emk212b7225kght-taiyo+yuden-29102998?r=sp</t>
+  </si>
+  <si>
+    <t>0805 2.2 uF 16 V ±10% Tolerance X7R Multilayer Ceramic Chip Capacitor</t>
   </si>
   <si>
     <t>ESDARF02-1BU2CK</t>
@@ -386,6 +434,12 @@
     <t>https://octopart.com/crgcq0402f10k-te+connectivity-91017932?r=sp</t>
   </si>
   <si>
+    <t>AC0402FR-073RL</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ac0402fr-073rl-yageo-71366773?r=sp</t>
+  </si>
+  <si>
     <t>R5</t>
   </si>
   <si>
@@ -437,6 +491,12 @@
     <t>Molex</t>
   </si>
   <si>
+    <t>https://octopart.com/0734120110-molex-16756629?r=sp&amp;s=MrVch9BMTneaw8n1KM-Tpw</t>
+  </si>
+  <si>
+    <t>Conn; RF/Coaxial; SMT; 50 Ohms; 1.25mm; Straight; Jack; Gold Plated</t>
+  </si>
+  <si>
     <t>U5</t>
   </si>
   <si>
@@ -455,6 +515,15 @@
     <t>https://octopart.com/teseo-liv3f-stmicroelectronics-84762432?r=sp</t>
   </si>
   <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>C5, C11</t>
+  </si>
+  <si>
+    <t>C10, C12, C19</t>
+  </si>
+  <si>
     <t>FB4</t>
   </si>
   <si>
@@ -476,88 +545,19 @@
     <t>0.0R DNP</t>
   </si>
   <si>
-    <t>C3, C5, C6, C8, C9</t>
-  </si>
-  <si>
-    <t>C4, C7</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>CGA2B3X7R1H103K050BE</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>https://octopart.com/cga2b3x7r1h103k050be-tdk-68305469?r=sp</t>
-  </si>
-  <si>
-    <t>Cap Ceramic 0.01uF 50V X7R 10% Pad SMD 0402 Soft Termination 125C Automotive T/R</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>AC0603FR-07100KL</t>
-  </si>
-  <si>
-    <t>https://octopart.com/ac0603fr-07100kl-yageo-21711090?r=sp</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>1.00uF</t>
-  </si>
-  <si>
-    <t>C0402C105K8PAC7411</t>
-  </si>
-  <si>
-    <t>Cap Ceramic 1uF 10V X5R 10% SMD 0402 85°C Paper T/R</t>
-  </si>
-  <si>
-    <t>https://octopart.com/c0402c105k8pac7411-kemet-75146233?r=sp</t>
-  </si>
-  <si>
-    <t>Cap Ceramic 2.2uF 4V X5R 10% SMD 0402 85°C Paper T/R</t>
-  </si>
-  <si>
-    <t>C0402C225K7PACTU</t>
-  </si>
-  <si>
-    <t>https://octopart.com/c0402c225k7pactu-kemet-89187402?r=sp</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C10, C19</t>
-  </si>
-  <si>
-    <t>Cap Ceramic 56pF 25V C0G 2% SMD 0201 125C Paper T/R</t>
-  </si>
-  <si>
-    <t>GRM0335C1E560GA01D</t>
-  </si>
-  <si>
-    <t>https://octopart.com/grm0335c1e560ga01d-murata-24611383?r=sp</t>
-  </si>
-  <si>
-    <t>732511150</t>
-  </si>
-  <si>
-    <t>https://octopart.com/73251-1150-molex-777272?r=sp</t>
-  </si>
-  <si>
-    <t>50 Ohms, SMA Jack Receptacle, Edge Mount, .25µm Gold (Au) Plating, One Piece Per Bag</t>
+    <t>3.0R DNP</t>
+  </si>
+  <si>
+    <t>2.2K</t>
+  </si>
+  <si>
+    <t>R15, R16</t>
+  </si>
+  <si>
+    <t>AC0402FR-072K2L</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ac0402fr-072k2l-yageo-24682183?r=sp</t>
   </si>
 </sst>
 </file>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,10 +982,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -997,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -1011,13 +1011,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1029,51 +1029,51 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G3" s="4">
         <v>0.1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4">
         <v>0.1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1081,47 +1081,47 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="2" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="2" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1129,23 +1129,23 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1153,23 +1153,25 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.1</v>
+      </c>
       <c r="H8" s="2" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1177,73 +1179,71 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>129</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="G9" s="4"/>
       <c r="H9" s="2" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0.1</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G10" s="4"/>
       <c r="H10" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="2" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1251,71 +1251,71 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>144</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G13" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="G13" s="1"/>
       <c r="H13" s="2" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="2" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1323,23 +1323,23 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="2" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1347,23 +1347,23 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="2" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1371,23 +1371,23 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="2" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1395,99 +1395,103 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="H18" s="2" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="H19" s="2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1495,51 +1499,51 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>133</v>
+        <v>29</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>134</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>148</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>26</v>
+        <v>150</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>27</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1547,23 +1551,23 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1571,49 +1575,49 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>149</v>
+      <c r="B26" s="1">
+        <v>734120110</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>149</v>
+        <v>128</v>
+      </c>
+      <c r="F26" s="1">
+        <v>734120110</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="2" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1627,7 +1631,7 @@
         <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>7</v>
@@ -1645,23 +1649,23 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="2" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1669,23 +1673,23 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="2" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1693,23 +1697,23 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="2" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1717,23 +1721,23 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="2" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1741,35 +1745,36 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1"/>
     <hyperlink ref="H4" r:id="rId2"/>
-    <hyperlink ref="H7" r:id="rId3"/>
-    <hyperlink ref="H15" r:id="rId4"/>
-    <hyperlink ref="H20" r:id="rId5"/>
-    <hyperlink ref="H21" r:id="rId6"/>
+    <hyperlink ref="H6" r:id="rId3"/>
+    <hyperlink ref="H12" r:id="rId4"/>
+    <hyperlink ref="H18" r:id="rId5"/>
+    <hyperlink ref="H19" r:id="rId6"/>
+    <hyperlink ref="H20" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Changing the layout design to improve the performance
</commit_message>
<xml_diff>
--- a/H1FR50/Released/BOM/H1FR50.xlsx
+++ b/H1FR50/Released/BOM/H1FR50.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H1FR50\H1FR50\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF1C5E4-95D1-4DDE-AC4A-2B10509CD810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918E813A-60D2-4B1A-A13E-B6747A5F8F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="360" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H21R00" sheetId="1" r:id="rId1"/>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1004,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>

</xml_diff>